<commit_message>
updated data.png, and data.xlsx, update images, updated README.md
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="12">
   <si>
     <t>CPU</t>
   </si>
@@ -51,11 +51,17 @@
   <si>
     <t>shared</t>
   </si>
+  <si>
+    <t>nobankconf</t>
+  </si>
+  <si>
+    <t>CPU(std::sort)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -65,7 +71,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -102,6 +108,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -115,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -123,6 +135,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -195,7 +208,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Time vs Size</a:t>
+              <a:t>Time vs Size Exponent</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -293,16 +306,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>2E-3</c:v>
+                  <c:v>8.0000000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>2.0699999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120</c:v>
+                  <c:v>32.200000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -372,10 +385,10 @@
                   <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>2.86</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54</c:v>
+                  <c:v>54.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -439,16 +452,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.27</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43</c:v>
+                  <c:v>0.28999999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>1.49</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>20</c:v>
+                  <c:v>20.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,8 +474,81 @@
           </c:extLst>
         </c:ser>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>shared</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$4:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$4:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8.9999999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.05</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C45A-4B49-9A5C-C4C36A93950C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:v>thrust</c:v>
           </c:tx>
@@ -507,21 +593,21 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$7</c:f>
+              <c:f>Sheet1!$G$4:$G$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.01</c:v>
+                  <c:v>1.4999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.89</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>0.67</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>4.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -788,10 +874,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.27928345297044055"/>
-          <c:y val="0.87950186841051647"/>
-          <c:w val="0.47641100274836773"/>
-          <c:h val="8.6599826504737742E-2"/>
+          <c:x val="9.526815142932564E-2"/>
+          <c:y val="0.8846172985602232"/>
+          <c:w val="0.82394835955508239"/>
+          <c:h val="9.5550498384233767E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -920,7 +1006,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Time vs Size</a:t>
+              <a:t>Time vs Size Exponent</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1018,16 +1104,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>3.0000000000000001E-3</c:v>
+                  <c:v>8.0000000000000004E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.75</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>160</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1091,16 +1177,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.24</c:v>
+                  <c:v>0.17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>29.05</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1109,6 +1195,79 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-E642-4476-83A6-EB79F4E3D95A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>shared</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$4:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$12:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E64C-478E-B8DB-14FA443B1369}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1367,10 +1526,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.39318426189373384"/>
-          <c:y val="0.9000104135873801"/>
-          <c:w val="0.26965388517611771"/>
-          <c:h val="7.0126105183950974E-2"/>
+          <c:x val="0.18374322293682752"/>
+          <c:y val="0.8904215146257719"/>
+          <c:w val="0.65113950832481815"/>
+          <c:h val="0.10250491367700763"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1499,11 +1658,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Time vs Size</a:t>
+              <a:t>Time vs Size Exponent</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.42615996501275977"/>
+          <c:y val="2.6595742358475807E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1597,16 +1764,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.03</c:v>
+                  <c:v>8.0000000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>87</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1285</c:v>
+                  <c:v>406</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1688,6 +1855,79 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6268-414A-A56C-E4C0EB4682A7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>shared</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="9525" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$4:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$E$20:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>220</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-66E5-4E32-89D2-EEA75568EF1E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1990,10 +2230,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.36793459576355775"/>
-          <c:y val="0.90214351938942772"/>
-          <c:w val="0.28349700565598313"/>
-          <c:h val="5.9460576173712074E-2"/>
+          <c:x val="0.19868433212315526"/>
+          <c:y val="0.90866472512853702"/>
+          <c:w val="0.69516425416882777"/>
+          <c:h val="6.256759767206492E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2011,7 +2251,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="lt1">
                   <a:lumMod val="75000"/>
@@ -3704,16 +3944,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>396240</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>589280</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>172720</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3742,16 +3982,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>274320</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>81280</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>35560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>213360</xdr:colOff>
-      <xdr:row>61</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3780,16 +4020,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>802640</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>40640</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>50800</xdr:colOff>
-      <xdr:row>55</xdr:row>
-      <xdr:rowOff>142240</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4081,17 +4321,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="12.5546875" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="6" width="13.5546875" customWidth="1"/>
@@ -4117,10 +4357,12 @@
       <c r="E2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -4138,100 +4380,116 @@
       <c r="E3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="6" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>2E-3</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="C4" s="2">
         <v>0.03</v>
       </c>
       <c r="D4" s="3">
-        <v>0.27</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="G4" s="4"/>
+        <v>0.13</v>
+      </c>
+      <c r="E4" s="5">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F4" s="7">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1.4999999999999999E-2</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>16</v>
       </c>
       <c r="B5" s="1">
-        <v>0.4</v>
+        <v>0.13</v>
       </c>
       <c r="C5" s="2">
         <v>0.13</v>
       </c>
       <c r="D5" s="3">
-        <v>0.43</v>
-      </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="6">
-        <v>0.89</v>
-      </c>
-      <c r="G5" s="4"/>
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="F5" s="7">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="G5" s="6">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>20</v>
       </c>
       <c r="B6" s="1">
-        <v>7</v>
+        <v>2.0699999999999998</v>
       </c>
       <c r="C6" s="2">
-        <v>2</v>
+        <v>2.86</v>
       </c>
       <c r="D6" s="3">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="6">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4"/>
+        <v>1.49</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="F6" s="7">
+        <v>0.63</v>
+      </c>
+      <c r="G6" s="6">
+        <v>0.67</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>24</v>
       </c>
       <c r="B7" s="1">
-        <v>120</v>
+        <v>32.200000000000003</v>
       </c>
       <c r="C7" s="2">
-        <v>54</v>
+        <v>54.2</v>
       </c>
       <c r="D7" s="3">
-        <v>20</v>
-      </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="6">
-        <v>4</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>20.8</v>
+      </c>
+      <c r="E7" s="5">
+        <v>9.14</v>
+      </c>
+      <c r="F7" s="7">
+        <v>9.48</v>
+      </c>
+      <c r="G7" s="6">
+        <v>4.2</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -4246,10 +4504,12 @@
       <c r="E10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="4"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -4267,88 +4527,96 @@
       <c r="E11" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G11" s="4"/>
+      <c r="G11" s="6" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12" s="1">
-        <v>3.0000000000000001E-3</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="3">
-        <v>0.24</v>
-      </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="4"/>
+        <v>0.17</v>
+      </c>
+      <c r="E12" s="5">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>16</v>
       </c>
       <c r="B13" s="1">
-        <v>0.75</v>
+        <v>0.18</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="4"/>
+        <v>0.35</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>20</v>
       </c>
       <c r="B14" s="1">
-        <v>12</v>
+        <v>2.8</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="3">
         <v>2</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="4"/>
+      <c r="E14" s="5">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="6"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>24</v>
       </c>
       <c r="B15" s="1">
-        <v>160</v>
+        <v>46</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="3">
-        <v>30</v>
-      </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="4"/>
+        <v>29.05</v>
+      </c>
+      <c r="E15" s="5">
+        <v>16.3</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>4</v>
@@ -4359,7 +4627,10 @@
       <c r="E18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="6" t="s">
         <v>3</v>
       </c>
     </row>
@@ -4379,7 +4650,10 @@
       <c r="E19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F19" s="6" t="s">
+      <c r="F19" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G19" s="6" t="s">
         <v>1</v>
       </c>
     </row>
@@ -4388,60 +4662,68 @@
         <v>8</v>
       </c>
       <c r="B20" s="1">
-        <v>0.03</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="3">
         <v>5</v>
       </c>
-      <c r="E20" s="5"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="4"/>
+      <c r="E20" s="5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="6"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>16</v>
       </c>
       <c r="B21" s="1">
-        <v>5</v>
+        <v>1.5</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="3">
         <v>6</v>
       </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="4"/>
+      <c r="E21" s="5">
+        <v>7</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="6"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
       <c r="B22" s="1">
-        <v>87</v>
+        <v>30</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="3">
         <v>30</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="4"/>
+      <c r="E22" s="5">
+        <v>24</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>24</v>
       </c>
       <c r="B23" s="1">
-        <v>1285</v>
+        <v>406</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="3">
         <v>369</v>
       </c>
-      <c r="E23" s="5"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="4"/>
+      <c r="E23" s="5">
+        <v>220</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G24" s="4"/>

</xml_diff>